<commit_message>
Fixed Fatal Flaw in RGB LED Data Line, Updated BOM
</commit_message>
<xml_diff>
--- a/BOM_total.xlsx
+++ b/BOM_total.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\keyboardv2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89D594F0-13F3-464D-90F5-0E0F3CBB9998}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47659A7D-DB09-4BD2-84F8-8EAD43C2A6E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
   <si>
     <t>Product/Item</t>
   </si>
@@ -135,6 +135,15 @@
   </si>
   <si>
     <t>Anti slip adhesive grips to apply to the back of the plastic</t>
+  </si>
+  <si>
+    <t>Meckeys</t>
+  </si>
+  <si>
+    <t>PCB Mounted</t>
+  </si>
+  <si>
+    <t>Stabilizers</t>
   </si>
 </sst>
 </file>
@@ -503,10 +512,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -661,31 +670,51 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9">
+        <v>1000</v>
+      </c>
+      <c r="D9">
+        <v>13</v>
+      </c>
+      <c r="E9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>25</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E10" t="s">
         <v>27</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="4">
-        <f>SUM(D2:D9)</f>
-        <v>140.93</v>
+      <c r="D11" s="4">
+        <f>SUM(D2:D10)</f>
+        <v>153.93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>